<commit_message>
Criando todos os VOs e DAOs 1 fase
</commit_message>
<xml_diff>
--- a/Concessionaria_Tabelas.xlsx
+++ b/Concessionaria_Tabelas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D17C4C-1B89-4065-95F4-F318CA56788B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4039E3-1796-4D6E-AFDA-E1EEB6F65FC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,6 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -71,9 +70,6 @@
     <t>TIPO_AUTOMOVEL</t>
   </si>
   <si>
-    <t>SEGURADORAS</t>
-  </si>
-  <si>
     <t>AUTOMOVEL</t>
   </si>
   <si>
@@ -207,6 +203,15 @@
   </si>
   <si>
     <t>DES_SENHA</t>
+  </si>
+  <si>
+    <t>SEGURADORA</t>
+  </si>
+  <si>
+    <t>DTA_FIM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUM_CPF_FUNCIONARIO &lt;FK&gt; </t>
   </si>
 </sst>
 </file>
@@ -223,7 +228,7 @@
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -561,7 +566,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,17 +605,17 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
@@ -618,31 +623,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -654,24 +659,24 @@
       </c>
       <c r="D5" s="2"/>
       <c r="I5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -683,30 +688,30 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>3</v>
@@ -717,33 +722,33 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="I14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>10</v>
@@ -754,13 +759,13 @@
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>13</v>
@@ -768,37 +773,40 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -812,63 +820,63 @@
         <v>9</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="G23" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="I24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CRUD v2 normalizando banco
</commit_message>
<xml_diff>
--- a/Concessionaria_Tabelas.xlsx
+++ b/Concessionaria_Tabelas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB75367A-40D0-4F81-82BC-DB911C063B83}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E7411D-6CBE-491C-818A-08A5DFF7DCE5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -70,9 +70,6 @@
     <t>ID_MODELO &lt;FK&gt;</t>
   </si>
   <si>
-    <t>ID_MARCA &lt;FK&gt;</t>
-  </si>
-  <si>
     <t>ID_COR &lt;FK&gt;</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>ID_TPAUTO &lt;FK&gt;</t>
   </si>
   <si>
-    <t>ID_MARCA &lt;FK&gt; &lt;PK&gt;</t>
-  </si>
-  <si>
     <t>NOM_MARCA</t>
   </si>
   <si>
@@ -154,9 +148,6 @@
     <t xml:space="preserve">DES_CHASSI &lt;PK&gt; </t>
   </si>
   <si>
-    <t>NUM_ANO &lt;PK&gt;</t>
-  </si>
-  <si>
     <t>NUM_TELEFONE</t>
   </si>
   <si>
@@ -199,9 +190,6 @@
     <t>DTA_NASCIMENTO</t>
   </si>
   <si>
-    <t>NUM_ANO&lt;FK&gt;</t>
-  </si>
-  <si>
     <t>DTA_VENDA&lt;PK&gt;</t>
   </si>
   <si>
@@ -215,6 +203,12 @@
   </si>
   <si>
     <t xml:space="preserve">ID_SEGURADORA &lt;FK&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUM_ANO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID_MARCA &lt;FK&gt; </t>
   </si>
 </sst>
 </file>
@@ -568,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,17 +602,17 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>10</v>
@@ -626,60 +620,60 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D5" s="2"/>
       <c r="I5" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -691,25 +685,25 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>3</v>
@@ -720,33 +714,33 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>9</v>
@@ -754,16 +748,16 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
@@ -771,42 +765,32 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -820,63 +804,63 @@
         <v>8</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G24" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="I25" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Versão Final do projeto Java + Scripts view e procedure
</commit_message>
<xml_diff>
--- a/Concessionaria_Tabelas.xlsx
+++ b/Concessionaria_Tabelas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A242932C-7829-4F2A-91C5-E817FF2D5201}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F185398-E792-412E-9675-8EB6BCE424C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>